<commit_message>
switched to streaming api
</commit_message>
<xml_diff>
--- a/realtime/realtime.xlsx
+++ b/realtime/realtime.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fz/Dev/xlwings-eikon/realtime/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felix\Dev\xlwings-eikon\realtime\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AB6A0C4-5AF5-CA48-BCEF-62A7E3CE7ABA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC090A59-EBBF-4E39-B23D-C9DED18FDDA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="820" yWindow="460" windowWidth="14960" windowHeight="18740" xr2:uid="{A3F4C8F7-A64B-E549-B14F-BF1F20928436}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13996" xr2:uid="{A3F4C8F7-A64B-E549-B14F-BF1F20928436}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,13 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>IBM</t>
-  </si>
-  <si>
-    <t>MSFT.O</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>CF_ASK</t>
   </si>
@@ -47,25 +41,37 @@
     <t>CF_BID</t>
   </si>
   <si>
-    <t>CF_LAST</t>
-  </si>
-  <si>
     <t>CF_TICK</t>
   </si>
   <si>
-    <t xml:space="preserve"> ⇩</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ⇧</t>
-  </si>
-  <si>
     <t>Instrument</t>
   </si>
   <si>
     <t xml:space="preserve">Last updated: </t>
   </si>
   <si>
-    <t>stopped</t>
+    <t>GBP=</t>
+  </si>
+  <si>
+    <t>JPY=</t>
+  </si>
+  <si>
+    <t>OPEN_PRC</t>
+  </si>
+  <si>
+    <t>CF_HIGH</t>
+  </si>
+  <si>
+    <t>CF_LOW</t>
+  </si>
+  <si>
+    <t>CF_CLOSE</t>
+  </si>
+  <si>
+    <t>CAD=</t>
+  </si>
+  <si>
+    <t>CHF=</t>
   </si>
 </sst>
 </file>
@@ -112,18 +118,171 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="20">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9B9B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9B9B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9B9B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9B9B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9B9B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9B9B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9B9B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9B9B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF9B9B"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -432,74 +591,148 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B8531DE-B935-5B4F-9F87-C249852EB155}">
-  <dimension ref="A1:E4"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.6875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="11.1875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="2">
-        <v>43946.663703703707</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="G2" s="4" t="s">
         <v>10</v>
       </c>
+      <c r="H2" s="4" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="4" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>124.72</v>
-      </c>
-      <c r="E3" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>174.5</v>
-      </c>
-      <c r="C4">
-        <v>174.4</v>
-      </c>
-      <c r="D4">
-        <v>174.55</v>
-      </c>
-      <c r="E4" t="s">
-        <v>7</v>
-      </c>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="H3">
+    <cfRule type="expression" dxfId="11" priority="23">
+      <formula>$H3=21</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="21">
+      <formula>$H3=22</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3:G3">
+    <cfRule type="expression" dxfId="8" priority="9">
+      <formula>$H3=22</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="10">
+      <formula>$H3=21</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H4:H6">
+    <cfRule type="expression" dxfId="6" priority="7">
+      <formula>$H4=22</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="7" priority="8">
+      <formula>$H4=21</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4:G6">
+    <cfRule type="expression" dxfId="5" priority="5">
+      <formula>$H4=22</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="6">
+      <formula>$H4=21</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A3">
+    <cfRule type="expression" dxfId="3" priority="3">
+      <formula>$H3=22</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="4">
+      <formula>$H3=21</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A4:A6">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>$H4=22</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="2">
+      <formula>$H4=21</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>